<commit_message>
adding Scenario for Components
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramkumar/T4S/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AAB64A-D7D5-3B44-B2B3-C8AA087866D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE11B05-BC24-3840-A08C-F2410A2D8BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="2880" windowWidth="25280" windowHeight="11320" xr2:uid="{2EBC4578-6CE2-44EC-9A0E-9864222B0DC3}"/>
+    <workbookView xWindow="680" yWindow="3920" windowWidth="25280" windowHeight="11320" activeTab="1" xr2:uid="{2EBC4578-6CE2-44EC-9A0E-9864222B0DC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -190,13 +190,43 @@
   </si>
   <si>
     <t>Automation1</t>
+  </si>
+  <si>
+    <t>Verify that user can add Breakdown for the component</t>
+  </si>
+  <si>
+    <t>Barbie Barbie Inc.</t>
+  </si>
+  <si>
+    <t>Tons</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>BreakdownMaterial</t>
+  </si>
+  <si>
+    <t>Synthetic Fibre</t>
+  </si>
+  <si>
+    <t>BreakdownSubMaterial</t>
+  </si>
+  <si>
+    <t>Rubber</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Algeria</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,12 +255,6 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -252,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -272,7 +296,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9761C36-153C-47B1-8C9F-40216D2A2F00}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -779,19 +802,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E73960C2-8A51-1B47-992E-18695F7796D5}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,17 +847,29 @@
         <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
@@ -844,6 +886,44 @@
       </c>
       <c r="H2" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding New scenario for Delete Breakdown and adding material link details
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramkumar/T4S/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE11B05-BC24-3840-A08C-F2410A2D8BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEE732D-0AAE-6E4D-8A55-405BA056F4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="3920" windowWidth="25280" windowHeight="11320" activeTab="1" xr2:uid="{2EBC4578-6CE2-44EC-9A0E-9864222B0DC3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -220,13 +220,43 @@
   </si>
   <si>
     <t>Algeria</t>
+  </si>
+  <si>
+    <t>Verify that user can link material for the product</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>TestProduct5</t>
+  </si>
+  <si>
+    <t>LM-MaterialName</t>
+  </si>
+  <si>
+    <t>LM-Wastage</t>
+  </si>
+  <si>
+    <t>LM-Unit</t>
+  </si>
+  <si>
+    <t>LM-Weight</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Verify that user can Delete Breakdown for the component</t>
+  </si>
+  <si>
+    <t>TC12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +285,18 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF3467E9"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -276,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -296,6 +338,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9761C36-153C-47B1-8C9F-40216D2A2F00}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -632,10 +676,12 @@
     <col min="22" max="22" width="8.6640625" style="4"/>
     <col min="23" max="23" width="14.5" style="4" customWidth="1"/>
     <col min="24" max="24" width="17.5" style="4" customWidth="1"/>
-    <col min="25" max="16384" width="8.6640625" style="4"/>
+    <col min="25" max="25" width="8.6640625" style="4"/>
+    <col min="26" max="26" width="19.1640625" style="4" customWidth="1"/>
+    <col min="27" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,8 +760,20 @@
       <c r="Z1" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -752,7 +810,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -775,23 +833,42 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB4">
+        <v>10</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
     </row>
@@ -802,10 +879,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E73960C2-8A51-1B47-992E-18695F7796D5}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -926,6 +1003,44 @@
         <v>100</v>
       </c>
     </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding New scenario for Document ruleset and Purchased order flow
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramkumar/T4S/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEE732D-0AAE-6E4D-8A55-405BA056F4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A482FF98-4A9F-D54C-8828-987DB13B99D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="3920" windowWidth="25280" windowHeight="11320" activeTab="1" xr2:uid="{2EBC4578-6CE2-44EC-9A0E-9864222B0DC3}"/>
+    <workbookView xWindow="1020" yWindow="2760" windowWidth="25280" windowHeight="11320" activeTab="2" xr2:uid="{2EBC4578-6CE2-44EC-9A0E-9864222B0DC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
     <sheet name="Component" sheetId="2" r:id="rId2"/>
+    <sheet name="DocumentRulesets" sheetId="3" r:id="rId3"/>
+    <sheet name="Orders" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="96">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -250,13 +252,88 @@
   </si>
   <si>
     <t>TC12</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>Document Type</t>
+  </si>
+  <si>
+    <t>Applies To</t>
+  </si>
+  <si>
+    <t>Audit Reports</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user can add a Ruleset </t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Purchase Processes</t>
+  </si>
+  <si>
+    <t>Ref No.</t>
+  </si>
+  <si>
+    <t>Secondary Supplier</t>
+  </si>
+  <si>
+    <t>Order Nature</t>
+  </si>
+  <si>
+    <t>External Customer Reference</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Testing2</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user can add a purchase Order </t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Tracing Template</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,18 +362,6 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF3467E9"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -318,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -338,8 +403,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9761C36-153C-47B1-8C9F-40216D2A2F00}">
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AE10" sqref="AE10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -780,8 +844,8 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E2" s="3"/>
@@ -817,10 +881,10 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -833,14 +897,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:30" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>63</v>
       </c>
       <c r="AA4" t="s">
@@ -881,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E73960C2-8A51-1B47-992E-18695F7796D5}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1044,4 +1109,198 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E16FFA-40B9-924E-BB0E-A3B4844A80F6}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="3" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352B204F-AEBE-5742-9A7D-8F1EB157B836}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2">
+        <v>123456</v>
+      </c>
+      <c r="H2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2">
+        <v>98765</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2">
+        <v>160</v>
+      </c>
+      <c r="O2" t="s">
+        <v>87</v>
+      </c>
+      <c r="P2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>